<commit_message>
Change plc code and add switch bounds
</commit_message>
<xml_diff>
--- a/TrainProject/Excel Files/TrackLayoutUpdated.xlsx
+++ b/TrainProject/Excel Files/TrackLayoutUpdated.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\Train-Project\TrainProject\TrainProject\Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabe\Documents\TrainProject\TrainProject\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="90">
   <si>
     <t>Block Number</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Z</t>
   </si>
   <si>
-    <t>SWITCH TO YARD</t>
-  </si>
-  <si>
     <t>SWITCH TO/FROM YARD</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
   </si>
   <si>
     <t>STATION; INGLEWOOD; UNDERGROUND</t>
-  </si>
-  <si>
-    <t>STATION; OVERBROOK; UNDERGROUND</t>
   </si>
   <si>
     <t>STATION; SWISSVILLE</t>
@@ -274,9 +268,6 @@
     <t>Head/Head</t>
   </si>
   <si>
-    <t>STATION; MT LEBANON</t>
-  </si>
-  <si>
     <t>STATION; NORTH POLE</t>
   </si>
   <si>
@@ -293,6 +284,12 @@
   </si>
   <si>
     <t>SWITCH; STATION; HERRON AVE</t>
+  </si>
+  <si>
+    <t>SWITCH TO YARD; STATION; OVERBROOK; UNDERGROUND</t>
+  </si>
+  <si>
+    <t>SWITCH; STATION; MT LEBANON</t>
   </si>
 </sst>
 </file>
@@ -720,23 +717,23 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:L78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="3"/>
-    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="3"/>
+    <col min="2" max="2" width="12.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="3" customWidth="1"/>
-    <col min="8" max="10" width="8.85546875" style="1"/>
-    <col min="11" max="11" width="10.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="10.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" style="3" customWidth="1"/>
+    <col min="8" max="10" width="8.81640625" style="1"/>
+    <col min="11" max="11" width="10.7265625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.26953125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -765,13 +762,13 @@
         <v>32</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -799,13 +796,13 @@
         <v>0.25</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Red</v>
@@ -834,7 +831,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A70" si="1">A3</f>
         <v>Red</v>
@@ -863,10 +860,10 @@
         <v>1.5</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -895,10 +892,10 @@
         <v>2.5</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -927,7 +924,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -956,10 +953,10 @@
         <v>3.75</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -991,10 +988,10 @@
         <v>4.125</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1023,7 +1020,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1044,7 +1041,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I10" s="8">
         <f t="shared" si="0"/>
@@ -1055,13 +1052,13 @@
         <v>4.125</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1090,13 +1087,13 @@
         <v>4.125</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1125,7 +1122,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1154,10 +1151,10 @@
         <v>3.375</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1186,10 +1183,10 @@
         <v>2.6909999999999998</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1218,7 +1215,7 @@
         <v>2.0909999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1250,13 +1247,13 @@
         <v>1.4909999999999997</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1288,13 +1285,13 @@
         <v>1.2409999999999997</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1323,7 +1320,7 @@
         <v>0.24099999999999966</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1353,7 +1350,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1382,7 +1379,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1411,10 +1408,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1435,7 +1432,7 @@
         <v>55</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I22" s="8">
         <f t="shared" si="0"/>
@@ -1446,10 +1443,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1478,7 +1475,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1507,10 +1504,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1542,10 +1539,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1577,7 +1574,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1609,7 +1606,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1641,10 +1638,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1676,10 +1673,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1711,7 +1708,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1743,7 +1740,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1775,7 +1772,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1807,10 +1804,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1842,10 +1839,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1877,7 +1874,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1909,7 +1906,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1941,7 +1938,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Red</v>
@@ -1973,7 +1970,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2005,10 +2002,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2040,10 +2037,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2075,7 +2072,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2107,7 +2104,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2139,7 +2136,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2171,10 +2168,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2206,10 +2203,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2241,10 +2238,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2276,10 +2273,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2300,7 +2297,7 @@
         <v>70</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I48" s="8">
         <f t="shared" si="0"/>
@@ -2311,7 +2308,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2343,10 +2340,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2375,10 +2372,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2407,7 +2404,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2436,7 +2433,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2468,10 +2465,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2500,10 +2497,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2532,10 +2529,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2564,10 +2561,10 @@
         <v>0.37499999999999967</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2596,7 +2593,7 @@
         <v>0.74999999999999967</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2625,10 +2622,10 @@
         <v>1.1249999999999996</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2657,10 +2654,10 @@
         <v>1.8749999999999996</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2689,7 +2686,7 @@
         <v>2.2499999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2721,10 +2718,10 @@
         <v>2.2499999999999996</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2753,10 +2750,10 @@
         <v>1.8749999999999996</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2785,7 +2782,7 @@
         <v>1.1249999999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2814,10 +2811,10 @@
         <v>0.37499999999999956</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2846,10 +2843,10 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2878,7 +2875,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2907,13 +2904,13 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2945,13 +2942,13 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2983,10 +2980,10 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3018,7 +3015,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="str">
         <f t="shared" ref="A71:A77" si="5">A70</f>
         <v>Red</v>
@@ -3050,10 +3047,10 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3085,13 +3082,13 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3123,13 +3120,13 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3161,10 +3158,10 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3196,7 +3193,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3228,10 +3225,10 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3263,13 +3260,13 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>10</v>
       </c>
@@ -3297,238 +3294,238 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C80" s="5"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C81" s="5"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C82" s="5"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C83" s="5"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C84" s="5"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C85" s="5"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C86" s="5"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C89" s="5"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C91" s="5"/>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C93" s="5"/>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C94" s="5"/>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C96" s="5"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C97" s="5"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C98" s="5"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C99" s="5"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C100" s="5"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C101" s="5"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C102" s="5"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C103" s="5"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C104" s="5"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C105" s="5"/>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C106" s="5"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C107" s="5"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C108" s="5"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C109" s="5"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C110" s="5"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C111" s="5"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C112" s="5"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C113" s="5"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C114" s="5"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C115" s="5"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C116" s="5"/>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C117" s="5"/>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C118" s="5"/>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C119" s="5"/>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C120" s="5"/>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C121" s="5"/>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C122" s="5"/>
     </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C123" s="5"/>
     </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C124" s="5"/>
     </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C125" s="5"/>
     </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C126" s="5"/>
     </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C127" s="5"/>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C128" s="5"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C129" s="5"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C130" s="5"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C131" s="5"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C132" s="5"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C133" s="5"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C134" s="5"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C135" s="5"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C136" s="5"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C137" s="5"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C138" s="5"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C139" s="5"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C140" s="5"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C141" s="5"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C142" s="5"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C143" s="5"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C144" s="5"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C145" s="5"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C146" s="5"/>
     </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C147" s="5"/>
     </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C148" s="5"/>
     </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C149" s="5"/>
     </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C150" s="5"/>
     </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C151" s="5"/>
     </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C152" s="5"/>
     </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C153" s="5"/>
     </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C154" s="5"/>
     </row>
   </sheetData>
@@ -3542,27 +3539,27 @@
   <dimension ref="A1:L230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G169" sqref="G169"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G168" sqref="G168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="3"/>
-    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="3"/>
+    <col min="2" max="2" width="12.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" style="3" customWidth="1"/>
     <col min="7" max="7" width="30" style="3" customWidth="1"/>
-    <col min="8" max="10" width="8.85546875" style="1"/>
-    <col min="11" max="11" width="8.85546875" style="3"/>
-    <col min="12" max="12" width="10.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="1"/>
+    <col min="8" max="10" width="8.81640625" style="1"/>
+    <col min="11" max="11" width="8.81640625" style="3"/>
+    <col min="12" max="12" width="10.81640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="32.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -3591,13 +3588,13 @@
         <v>32</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -3625,13 +3622,13 @@
         <v>0.5</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Green</v>
@@ -3652,7 +3649,7 @@
         <v>55</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I66" si="0">E3*D3/100</f>
@@ -3663,7 +3660,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A70" si="1">A3</f>
         <v>Green</v>
@@ -3692,10 +3689,10 @@
         <v>3</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3724,10 +3721,10 @@
         <v>5</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3756,7 +3753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3785,10 +3782,10 @@
         <v>12</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3818,10 +3815,10 @@
         <v>17</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3850,7 +3847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3871,7 +3868,7 @@
         <v>55</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
@@ -3882,7 +3879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3911,7 +3908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3940,7 +3937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3960,9 +3957,6 @@
       <c r="F13" s="3">
         <v>55</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="I13" s="3">
         <f t="shared" si="0"/>
         <v>-3</v>
@@ -3972,13 +3966,13 @@
         <v>0</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3998,6 +3992,9 @@
       <c r="F14" s="3">
         <v>70</v>
       </c>
+      <c r="G14" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4007,13 +4004,13 @@
         <v>0</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4042,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4071,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4092,7 +4089,7 @@
         <v>70</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="0"/>
@@ -4103,10 +4100,10 @@
         <v>0</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4135,10 +4132,10 @@
         <v>0</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4167,7 +4164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4188,7 +4185,7 @@
         <v>60</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="0"/>
@@ -4199,7 +4196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4228,10 +4225,10 @@
         <v>0</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4260,10 +4257,10 @@
         <v>0</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4284,7 +4281,7 @@
         <v>70</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="0"/>
@@ -4295,7 +4292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4324,7 +4321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4353,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4382,7 +4379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4411,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4440,7 +4437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4460,6 +4457,9 @@
       <c r="F29" s="3">
         <v>70</v>
       </c>
+      <c r="G29" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I29" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4469,13 +4469,13 @@
         <v>0</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4495,9 +4495,6 @@
       <c r="F30" s="3">
         <v>70</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="I30" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4507,13 +4504,13 @@
         <v>0</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4542,7 +4539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4563,7 +4560,7 @@
         <v>70</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I32" s="3">
         <f t="shared" si="0"/>
@@ -4574,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4603,10 +4600,10 @@
         <v>0</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4635,10 +4632,10 @@
         <v>0</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4667,7 +4664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4696,10 +4693,10 @@
         <v>0</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4731,10 +4728,10 @@
         <v>0</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Green</v>
@@ -4766,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4798,7 +4795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4819,7 +4816,7 @@
         <v>70</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I40" s="3">
         <f t="shared" si="0"/>
@@ -4830,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4862,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4894,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4926,7 +4923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4958,7 +4955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4990,7 +4987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5022,7 +5019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5054,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5086,7 +5083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5107,7 +5104,7 @@
         <v>70</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I49" s="3">
         <f t="shared" si="0"/>
@@ -5118,7 +5115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5150,7 +5147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5182,7 +5179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5214,7 +5211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5246,7 +5243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5278,7 +5275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5310,7 +5307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5342,7 +5339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5374,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5395,7 +5392,7 @@
         <v>70</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="0"/>
@@ -5406,13 +5403,13 @@
         <v>0</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5432,9 +5429,7 @@
       <c r="F59" s="3">
         <v>60</v>
       </c>
-      <c r="G59" s="7" t="s">
-        <v>47</v>
-      </c>
+      <c r="G59" s="7"/>
       <c r="I59" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5444,13 +5439,13 @@
         <v>0</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5479,7 +5474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5508,7 +5503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5537,10 +5532,10 @@
         <v>0</v>
       </c>
       <c r="K62" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5561,7 +5556,7 @@
         <v>60</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I63" s="3">
         <f t="shared" si="0"/>
@@ -5572,13 +5567,13 @@
         <v>0</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5607,10 +5602,10 @@
         <v>0</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5639,7 +5634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5660,7 +5655,7 @@
         <v>70</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I66" s="3">
         <f t="shared" si="0"/>
@@ -5671,7 +5666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5700,7 +5695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5729,7 +5724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5758,10 +5753,10 @@
         <v>0</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5790,10 +5785,10 @@
         <v>0</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="str">
         <f t="shared" ref="A71:A134" si="5">A70</f>
         <v>Green</v>
@@ -5822,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5851,7 +5846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5880,7 +5875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5901,7 +5896,7 @@
         <v>60</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I74" s="3">
         <f t="shared" si="3"/>
@@ -5912,10 +5907,10 @@
         <v>0</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5944,10 +5939,10 @@
         <v>0</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5976,7 +5971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5996,9 +5991,6 @@
       <c r="F77" s="3">
         <v>60</v>
       </c>
-      <c r="G77" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="I77" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -6008,13 +6000,13 @@
         <v>0</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6035,7 +6027,7 @@
         <v>70</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="I78" s="3">
         <f t="shared" ref="I78:I109" si="6">E78*D78/100</f>
@@ -6046,13 +6038,13 @@
         <v>0</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6081,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6110,7 +6102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6139,7 +6131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6168,7 +6160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6197,7 +6189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6226,7 +6218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6255,7 +6247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6275,6 +6267,9 @@
       <c r="F86" s="3">
         <v>70</v>
       </c>
+      <c r="G86" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I86" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -6284,13 +6279,13 @@
         <v>0</v>
       </c>
       <c r="K86" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6310,9 +6305,6 @@
       <c r="F87" s="3">
         <v>55</v>
       </c>
-      <c r="G87" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="I87" s="3">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -6322,13 +6314,13 @@
         <v>0</v>
       </c>
       <c r="K87" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6357,7 +6349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6378,7 +6370,7 @@
         <v>55</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I89" s="3">
         <f t="shared" si="6"/>
@@ -6389,10 +6381,10 @@
         <v>0</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6421,10 +6413,10 @@
         <v>-0.375</v>
       </c>
       <c r="L90" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6453,7 +6445,7 @@
         <v>-1.125</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6482,7 +6474,7 @@
         <v>-2.625</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6511,7 +6503,7 @@
         <v>-2.625</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6540,7 +6532,7 @@
         <v>-1.125</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6569,7 +6561,7 @@
         <v>-0.375</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6598,7 +6590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6619,7 +6611,7 @@
         <v>55</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I97" s="3">
         <f t="shared" si="6"/>
@@ -6630,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6659,10 +6651,10 @@
         <v>0</v>
       </c>
       <c r="L98" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6691,10 +6683,10 @@
         <v>0</v>
       </c>
       <c r="L99" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6723,7 +6715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6752,13 +6744,13 @@
         <v>0</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L101" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6787,13 +6779,13 @@
         <v>0</v>
       </c>
       <c r="K102" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L102" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6822,10 +6814,10 @@
         <v>0</v>
       </c>
       <c r="L103" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6854,7 +6846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6883,10 +6875,10 @@
         <v>0</v>
       </c>
       <c r="L105" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6919,10 +6911,10 @@
         <v>0</v>
       </c>
       <c r="L106" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6951,7 +6943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6980,7 +6972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7009,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7038,10 +7030,10 @@
         <v>0</v>
       </c>
       <c r="L110" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7070,10 +7062,10 @@
         <v>0</v>
       </c>
       <c r="L111" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7102,7 +7094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7131,7 +7123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7160,7 +7152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7193,7 +7185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7222,7 +7214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7251,10 +7243,10 @@
         <v>0</v>
       </c>
       <c r="L117" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7283,10 +7275,10 @@
         <v>0</v>
       </c>
       <c r="L118" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7315,7 +7307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7344,7 +7336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7373,7 +7365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7402,10 +7394,10 @@
         <v>0</v>
       </c>
       <c r="L122" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7437,10 +7429,10 @@
         <v>0</v>
       </c>
       <c r="L123" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7462,7 +7454,7 @@
       </c>
       <c r="G124" s="7" t="str">
         <f>G58</f>
-        <v>STATION; OVERBROOK; UNDERGROUND</v>
+        <v>SWITCH TO YARD; STATION; OVERBROOK; UNDERGROUND</v>
       </c>
       <c r="I124" s="3">
         <f t="shared" si="8"/>
@@ -7473,7 +7465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7505,7 +7497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7537,7 +7529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7569,7 +7561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7601,7 +7593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7633,7 +7625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7665,7 +7657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7697,7 +7689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7729,7 +7721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7762,7 +7754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7794,7 +7786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="str">
         <f t="shared" ref="A135:A153" si="10">A134</f>
         <v>Green</v>
@@ -7826,7 +7818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7858,7 +7850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7890,7 +7882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7922,7 +7914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7954,7 +7946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7986,7 +7978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8018,7 +8010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8051,7 +8043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8083,7 +8075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8115,10 +8107,10 @@
         <v>0</v>
       </c>
       <c r="L144" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8147,10 +8139,10 @@
         <v>0</v>
       </c>
       <c r="L145" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8179,7 +8171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8208,10 +8200,10 @@
         <v>0</v>
       </c>
       <c r="L147" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8240,10 +8232,10 @@
         <v>0</v>
       </c>
       <c r="L148" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A149" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8272,7 +8264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8301,10 +8293,10 @@
         <v>0</v>
       </c>
       <c r="L150" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A151" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8333,19 +8325,19 @@
         <v>0</v>
       </c>
       <c r="K151" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L151" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C152" s="5">
         <v>151</v>
@@ -8368,19 +8360,19 @@
         <v>0</v>
       </c>
       <c r="K152" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L152" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A153" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C153" s="5">
         <v>152</v>
@@ -8403,13 +8395,13 @@
         <v>0</v>
       </c>
       <c r="K153" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L153" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" s="3" t="s">
         <v>10</v>
       </c>
@@ -8437,13 +8429,13 @@
         <v>0.25</v>
       </c>
       <c r="K154" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L154" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A155" s="3" t="str">
         <f>A154</f>
         <v>Red</v>
@@ -8472,7 +8464,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" s="3" t="str">
         <f t="shared" ref="A156:A219" si="14">A155</f>
         <v>Red</v>
@@ -8501,10 +8493,10 @@
         <v>1.5</v>
       </c>
       <c r="L156" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A157" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8533,10 +8525,10 @@
         <v>2.5</v>
       </c>
       <c r="L157" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8565,7 +8557,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A159" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8594,10 +8586,10 @@
         <v>3.75</v>
       </c>
       <c r="L159" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8618,7 +8610,7 @@
         <v>40</v>
       </c>
       <c r="G160" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I160" s="8">
         <f t="shared" si="13"/>
@@ -8629,10 +8621,10 @@
         <v>4.125</v>
       </c>
       <c r="L160" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A161" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8661,7 +8653,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A162" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8682,7 +8674,7 @@
         <v>40</v>
       </c>
       <c r="G162" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I162" s="8">
         <f t="shared" si="13"/>
@@ -8693,13 +8685,13 @@
         <v>4.125</v>
       </c>
       <c r="K162" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L162" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A163" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8728,13 +8720,13 @@
         <v>4.125</v>
       </c>
       <c r="K163" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L163" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A164" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8763,7 +8755,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A165" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8792,10 +8784,10 @@
         <v>3.375</v>
       </c>
       <c r="L165" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A166" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8824,10 +8816,10 @@
         <v>2.6909999999999998</v>
       </c>
       <c r="L166" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A167" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8856,7 +8848,7 @@
         <v>2.0909999999999997</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A168" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8885,13 +8877,13 @@
         <v>1.4909999999999997</v>
       </c>
       <c r="K168" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L168" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="169" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A169" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8912,7 +8904,7 @@
         <v>40</v>
       </c>
       <c r="G169" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I169" s="8">
         <f t="shared" si="13"/>
@@ -8923,13 +8915,13 @@
         <v>1.2409999999999997</v>
       </c>
       <c r="K169" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L169" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A170" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8958,7 +8950,7 @@
         <v>0.24099999999999966</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A171" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8988,7 +8980,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A172" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9017,7 +9009,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A173" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9046,10 +9038,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L173" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A174" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9070,7 +9062,7 @@
         <v>55</v>
       </c>
       <c r="G174" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I174" s="8">
         <f t="shared" si="13"/>
@@ -9081,10 +9073,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L174" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A175" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9113,7 +9105,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A176" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9142,10 +9134,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L176" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A177" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9177,10 +9169,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L177" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="178" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A178" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9201,7 +9193,7 @@
         <v>70</v>
       </c>
       <c r="G178" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I178" s="8">
         <f t="shared" si="13"/>
@@ -9212,7 +9204,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A179" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9244,7 +9236,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A180" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9276,10 +9268,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K180" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A181" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9311,10 +9303,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K181" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A182" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9346,7 +9338,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A183" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9378,7 +9370,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A184" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9410,7 +9402,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A185" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9442,10 +9434,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K185" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A186" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9477,10 +9469,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K186" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A187" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9512,7 +9504,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="188" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A188" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9533,7 +9525,7 @@
         <v>70</v>
       </c>
       <c r="G188" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I188" s="8">
         <f t="shared" si="13"/>
@@ -9544,7 +9536,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A189" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9576,7 +9568,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A190" s="3" t="str">
         <f>A186</f>
         <v>Red</v>
@@ -9608,7 +9600,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A191" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9640,10 +9632,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K191" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A192" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9675,10 +9667,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K192" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A193" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9710,7 +9702,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9742,7 +9734,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A195" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9774,7 +9766,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9795,7 +9787,7 @@
         <v>70</v>
       </c>
       <c r="G196" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I196" s="8">
         <f t="shared" si="13"/>
@@ -9806,10 +9798,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K196" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A197" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9830,7 +9822,7 @@
         <v>70</v>
       </c>
       <c r="G197" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I197" s="8">
         <f t="shared" si="13"/>
@@ -9841,10 +9833,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K197" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="198" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A198" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9865,7 +9857,7 @@
         <v>70</v>
       </c>
       <c r="G198" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I198" s="8">
         <f t="shared" si="13"/>
@@ -9876,10 +9868,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L198" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A199" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9911,10 +9903,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L199" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9935,7 +9927,7 @@
         <v>70</v>
       </c>
       <c r="G200" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I200" s="8">
         <f t="shared" si="13"/>
@@ -9946,7 +9938,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A201" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9978,10 +9970,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L201" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10010,10 +10002,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L202" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A203" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10042,7 +10034,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A204" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10071,7 +10063,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A205" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10103,10 +10095,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K205" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A206" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10135,10 +10127,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="K206" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A207" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10167,10 +10159,10 @@
         <v>-3.3306690738754696E-16</v>
       </c>
       <c r="L207" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A208" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10199,10 +10191,10 @@
         <v>0.37499999999999967</v>
       </c>
       <c r="L208" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A209" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10231,7 +10223,7 @@
         <v>0.74999999999999967</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A210" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10260,10 +10252,10 @@
         <v>1.1249999999999996</v>
       </c>
       <c r="L210" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A211" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10292,10 +10284,10 @@
         <v>1.8749999999999996</v>
       </c>
       <c r="L211" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A212" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10324,7 +10316,7 @@
         <v>2.2499999999999996</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A213" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10356,10 +10348,10 @@
         <v>2.2499999999999996</v>
       </c>
       <c r="L213" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A214" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10388,10 +10380,10 @@
         <v>1.8749999999999996</v>
       </c>
       <c r="L214" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A215" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10420,7 +10412,7 @@
         <v>1.1249999999999996</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A216" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10449,10 +10441,10 @@
         <v>0.37499999999999956</v>
       </c>
       <c r="L216" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A217" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10481,10 +10473,10 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="L217" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A218" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10513,7 +10505,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A219" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10542,13 +10534,13 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K219" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L219" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A220" s="3" t="str">
         <f t="shared" ref="A220:A229" si="17">A219</f>
         <v>Red</v>
@@ -10580,13 +10572,13 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K220" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L220" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A221" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10618,10 +10610,10 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="L221" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A222" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10653,7 +10645,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A223" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10685,10 +10677,10 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="L223" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A224" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10720,13 +10712,13 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K224" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L224" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A225" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10758,13 +10750,13 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K225" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L225" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A226" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10796,10 +10788,10 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="L226" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A227" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10831,7 +10823,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A228" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10863,10 +10855,10 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="L228" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A229" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10898,13 +10890,13 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K229" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L229" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A230" s="3" t="s">
         <v>10</v>
       </c>
@@ -10932,10 +10924,10 @@
         <v>-4.4408920985006262E-16</v>
       </c>
       <c r="K230" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L230" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PLC bug fixes and other changes
</commit_message>
<xml_diff>
--- a/TrainProject/Excel Files/TrackLayoutUpdated.xlsx
+++ b/TrainProject/Excel Files/TrackLayoutUpdated.xlsx
@@ -3539,8 +3539,8 @@
   <dimension ref="A1:L230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G168" sqref="G168"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed broken blocks, some plc logic. Switch table shows block numbers
</commit_message>
<xml_diff>
--- a/TrainProject/Excel Files/TrackLayoutUpdated.xlsx
+++ b/TrainProject/Excel Files/TrackLayoutUpdated.xlsx
@@ -3539,8 +3539,8 @@
   <dimension ref="A1:L230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G196" sqref="G196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9423,7 +9423,7 @@
         <v>70</v>
       </c>
       <c r="G185" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I185" s="8">
         <f t="shared" si="13"/>
@@ -9458,7 +9458,7 @@
         <v>70</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I186" s="8">
         <f t="shared" si="13"/>
@@ -9787,7 +9787,7 @@
         <v>70</v>
       </c>
       <c r="G196" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I196" s="8">
         <f t="shared" si="13"/>
@@ -9822,7 +9822,7 @@
         <v>70</v>
       </c>
       <c r="G197" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I197" s="8">
         <f t="shared" si="13"/>

</xml_diff>

<commit_message>
Finished commenting code and made it so you can enter kp and ki if you want, if not they have default values
</commit_message>
<xml_diff>
--- a/TrainProject/Excel Files/TrackLayoutUpdated.xlsx
+++ b/TrainProject/Excel Files/TrackLayoutUpdated.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabe\Documents\TrainProject\TrainProject\Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naran\Desktop\Trainzzz\TrainProject\TrainProject\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -717,23 +717,23 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:L78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="3"/>
-    <col min="2" max="2" width="12.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="3"/>
+    <col min="2" max="2" width="12.796875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" style="3" customWidth="1"/>
-    <col min="8" max="10" width="8.81640625" style="1"/>
-    <col min="11" max="11" width="10.7265625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.26953125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.453125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.81640625" style="1"/>
+    <col min="5" max="5" width="10.53125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.265625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.46484375" style="3" customWidth="1"/>
+    <col min="8" max="10" width="8.796875" style="1"/>
+    <col min="11" max="11" width="10.73046875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.265625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.46484375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -768,7 +768,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -802,7 +802,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Red</v>
@@ -831,7 +831,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A70" si="1">A3</f>
         <v>Red</v>
@@ -863,7 +863,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -895,7 +895,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -924,7 +924,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -956,7 +956,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -991,7 +991,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1020,7 +1020,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1058,7 +1058,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1093,7 +1093,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1122,7 +1122,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1154,7 +1154,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1186,7 +1186,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1215,7 +1215,7 @@
         <v>2.0909999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1253,7 +1253,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1291,7 +1291,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1320,7 +1320,7 @@
         <v>0.24099999999999966</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1350,7 +1350,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1379,7 +1379,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1411,7 +1411,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1446,7 +1446,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1475,7 +1475,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1507,7 +1507,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1542,7 +1542,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1574,7 +1574,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1606,7 +1606,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1641,7 +1641,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A29" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1676,7 +1676,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1708,7 +1708,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1740,7 +1740,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1772,7 +1772,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1807,7 +1807,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1842,7 +1842,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1874,7 +1874,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1906,7 +1906,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1938,7 +1938,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Red</v>
@@ -1970,7 +1970,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A39" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2005,7 +2005,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2040,7 +2040,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2072,7 +2072,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2104,7 +2104,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2136,7 +2136,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2171,7 +2171,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2206,7 +2206,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2241,7 +2241,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2276,7 +2276,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2308,7 +2308,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2343,7 +2343,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2375,7 +2375,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2404,7 +2404,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A52" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2433,7 +2433,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2468,7 +2468,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A54" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2500,7 +2500,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A55" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2532,7 +2532,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A56" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2564,7 +2564,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A57" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2593,7 +2593,7 @@
         <v>0.74999999999999967</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A58" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2625,7 +2625,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A59" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2657,7 +2657,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A60" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2686,7 +2686,7 @@
         <v>2.2499999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A61" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2721,7 +2721,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A62" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2753,7 +2753,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A63" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2782,7 +2782,7 @@
         <v>1.1249999999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A64" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2814,7 +2814,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A65" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2846,7 +2846,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2875,7 +2875,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A67" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2910,7 +2910,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A68" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2948,7 +2948,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2983,7 +2983,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3015,7 +3015,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A71" s="3" t="str">
         <f t="shared" ref="A71:A77" si="5">A70</f>
         <v>Red</v>
@@ -3050,7 +3050,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A72" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3088,7 +3088,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A73" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3126,7 +3126,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A74" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3161,7 +3161,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3193,7 +3193,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3228,7 +3228,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A77" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3266,7 +3266,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A78" s="3" t="s">
         <v>10</v>
       </c>
@@ -3300,232 +3300,232 @@
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.5">
       <c r="C79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.5">
       <c r="C80" s="5"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C81" s="5"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C82" s="5"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C83" s="5"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C84" s="5"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C85" s="5"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C86" s="5"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C89" s="5"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C91" s="5"/>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C93" s="5"/>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C94" s="5"/>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C96" s="5"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C97" s="5"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C98" s="5"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C99" s="5"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C100" s="5"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C101" s="5"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C102" s="5"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C103" s="5"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C104" s="5"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C105" s="5"/>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C106" s="5"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C107" s="5"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C108" s="5"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C109" s="5"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C110" s="5"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C111" s="5"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C112" s="5"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C113" s="5"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C114" s="5"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C115" s="5"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C116" s="5"/>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C117" s="5"/>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C118" s="5"/>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C119" s="5"/>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C120" s="5"/>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C121" s="5"/>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C122" s="5"/>
     </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C123" s="5"/>
     </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C124" s="5"/>
     </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C125" s="5"/>
     </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C126" s="5"/>
     </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C127" s="5"/>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C128" s="5"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C129" s="5"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C130" s="5"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C131" s="5"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C132" s="5"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C133" s="5"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C134" s="5"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C135" s="5"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C136" s="5"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C137" s="5"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C138" s="5"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C139" s="5"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C140" s="5"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C141" s="5"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C142" s="5"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C143" s="5"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C144" s="5"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C145" s="5"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C146" s="5"/>
     </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C147" s="5"/>
     </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C148" s="5"/>
     </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C149" s="5"/>
     </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C150" s="5"/>
     </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C151" s="5"/>
     </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C152" s="5"/>
     </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C153" s="5"/>
     </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C154" s="5"/>
     </row>
   </sheetData>
@@ -3539,27 +3539,27 @@
   <dimension ref="A1:L230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G196" sqref="G196"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="3"/>
-    <col min="2" max="2" width="12.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="3"/>
+    <col min="2" max="2" width="12.796875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.53125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.265625" style="3" customWidth="1"/>
     <col min="7" max="7" width="30" style="3" customWidth="1"/>
-    <col min="8" max="10" width="8.81640625" style="1"/>
-    <col min="11" max="11" width="8.81640625" style="3"/>
-    <col min="12" max="12" width="10.81640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.453125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.81640625" style="1"/>
+    <col min="8" max="10" width="8.796875" style="1"/>
+    <col min="11" max="11" width="8.796875" style="3"/>
+    <col min="12" max="12" width="10.796875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.46484375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="32.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="32.65" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Green</v>
@@ -3660,7 +3660,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A70" si="1">A3</f>
         <v>Green</v>
@@ -3692,7 +3692,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3724,7 +3724,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3753,7 +3753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3785,7 +3785,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3818,7 +3818,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3847,7 +3847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3879,7 +3879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3908,7 +3908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3937,7 +3937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3972,7 +3972,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4010,7 +4010,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4039,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4068,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4103,7 +4103,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4135,7 +4135,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4164,7 +4164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4196,7 +4196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4228,7 +4228,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4260,7 +4260,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4292,7 +4292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4321,7 +4321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4350,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4379,7 +4379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4408,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4437,7 +4437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A29" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4475,7 +4475,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4510,7 +4510,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4539,7 +4539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4571,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4603,7 +4603,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4635,7 +4635,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4664,7 +4664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4696,7 +4696,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4731,7 +4731,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Green</v>
@@ -4763,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A39" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4795,7 +4795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4827,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4859,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4891,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4923,7 +4923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4955,7 +4955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4987,7 +4987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5019,7 +5019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5051,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5083,7 +5083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5115,7 +5115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5147,7 +5147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5179,7 +5179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A52" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5211,7 +5211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5243,7 +5243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A54" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5275,7 +5275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A55" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5307,7 +5307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A56" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5339,7 +5339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A57" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5371,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A58" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5409,7 +5409,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A59" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5445,7 +5445,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A60" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5474,7 +5474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A61" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5503,7 +5503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A62" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5531,11 +5531,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K62" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A63" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5555,9 +5552,6 @@
       <c r="F63" s="3">
         <v>60</v>
       </c>
-      <c r="G63" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="I63" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5573,7 +5567,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A64" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5593,6 +5587,9 @@
       <c r="F64" s="3">
         <v>70</v>
       </c>
+      <c r="G64" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="I64" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5600,12 +5597,15 @@
       <c r="J64" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="L64" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A65" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5634,7 +5634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5666,7 +5666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A67" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5695,7 +5695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A68" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5724,7 +5724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5756,7 +5756,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5788,7 +5788,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A71" s="3" t="str">
         <f t="shared" ref="A71:A134" si="5">A70</f>
         <v>Green</v>
@@ -5817,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A72" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5846,7 +5846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A73" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5875,7 +5875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A74" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5910,7 +5910,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5942,7 +5942,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5971,7 +5971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A77" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6006,7 +6006,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A78" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6044,7 +6044,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A79" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6073,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A80" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6102,7 +6102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A81" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6131,7 +6131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A82" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6160,7 +6160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A83" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6189,7 +6189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A84" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6218,7 +6218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A85" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6247,7 +6247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A86" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6285,7 +6285,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A87" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6320,7 +6320,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A88" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6349,7 +6349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A89" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6384,7 +6384,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A90" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6416,7 +6416,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A91" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6445,7 +6445,7 @@
         <v>-1.125</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A92" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6474,7 +6474,7 @@
         <v>-2.625</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A93" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6503,7 +6503,7 @@
         <v>-2.625</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A94" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6532,7 +6532,7 @@
         <v>-1.125</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A95" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6561,7 +6561,7 @@
         <v>-0.375</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A96" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6590,7 +6590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A97" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6622,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A98" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6654,7 +6654,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A99" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6686,7 +6686,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A100" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6715,7 +6715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A101" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6750,7 +6750,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A102" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6785,7 +6785,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A103" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6817,7 +6817,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A104" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6846,7 +6846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A105" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6878,7 +6878,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A106" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6914,7 +6914,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A107" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6943,7 +6943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A108" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6972,7 +6972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A109" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7001,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A110" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7033,7 +7033,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A111" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7065,7 +7065,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A112" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7094,7 +7094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A113" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7123,7 +7123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A114" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7152,7 +7152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A115" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7185,7 +7185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A116" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7214,7 +7214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A117" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7246,7 +7246,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A118" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7278,7 +7278,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A119" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7307,7 +7307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A120" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7336,7 +7336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A121" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7365,7 +7365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A122" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7397,7 +7397,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A123" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7432,7 +7432,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A124" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7465,7 +7465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A125" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7497,7 +7497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A126" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7529,7 +7529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A127" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7561,7 +7561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A128" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7593,7 +7593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A129" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7625,7 +7625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A130" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7657,7 +7657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A131" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7689,7 +7689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A132" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7721,7 +7721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A133" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7754,7 +7754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A134" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7786,7 +7786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A135" s="3" t="str">
         <f t="shared" ref="A135:A153" si="10">A134</f>
         <v>Green</v>
@@ -7818,7 +7818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A136" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7850,7 +7850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A137" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7882,7 +7882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A138" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7914,7 +7914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A139" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7946,7 +7946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A140" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7978,7 +7978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A141" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8010,7 +8010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A142" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8043,7 +8043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A143" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8075,7 +8075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A144" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8110,7 +8110,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A145" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8142,7 +8142,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A146" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8171,7 +8171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A147" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8203,7 +8203,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A148" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8235,7 +8235,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A149" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8264,7 +8264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A150" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8296,7 +8296,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A151" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8331,7 +8331,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A152" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8366,7 +8366,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A153" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8401,7 +8401,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A154" s="3" t="s">
         <v>10</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A155" s="3" t="str">
         <f>A154</f>
         <v>Red</v>
@@ -8464,7 +8464,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A156" s="3" t="str">
         <f t="shared" ref="A156:A219" si="14">A155</f>
         <v>Red</v>
@@ -8496,7 +8496,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A157" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8528,7 +8528,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A158" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8557,7 +8557,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A159" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8589,7 +8589,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A160" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8624,7 +8624,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A161" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8653,7 +8653,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A162" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8691,7 +8691,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A163" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8726,7 +8726,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A164" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8755,7 +8755,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A165" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8787,7 +8787,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A166" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8819,7 +8819,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A167" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8848,7 +8848,7 @@
         <v>2.0909999999999997</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A168" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8883,7 +8883,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="169" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A169" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8921,7 +8921,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A170" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8950,7 +8950,7 @@
         <v>0.24099999999999966</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A171" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8980,7 +8980,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A172" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9009,7 +9009,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A173" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9041,7 +9041,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A174" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9076,7 +9076,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A175" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9105,7 +9105,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A176" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9137,7 +9137,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A177" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9172,7 +9172,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A178" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9204,7 +9204,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A179" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9236,7 +9236,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A180" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9271,7 +9271,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A181" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9306,7 +9306,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A182" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9338,7 +9338,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A183" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9370,7 +9370,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A184" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9402,7 +9402,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A185" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9437,7 +9437,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A186" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9472,7 +9472,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A187" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9504,7 +9504,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="188" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A188" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9536,7 +9536,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A189" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9568,7 +9568,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A190" s="3" t="str">
         <f>A186</f>
         <v>Red</v>
@@ -9600,7 +9600,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A191" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9635,7 +9635,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A192" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9670,7 +9670,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A193" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9702,7 +9702,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A194" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9734,7 +9734,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A195" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9766,7 +9766,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A196" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9801,7 +9801,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A197" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9836,7 +9836,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="198" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A198" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9871,7 +9871,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A199" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9906,7 +9906,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A200" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9938,7 +9938,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A201" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9973,7 +9973,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A202" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10005,7 +10005,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A203" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10034,7 +10034,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A204" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10063,7 +10063,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A205" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10098,7 +10098,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A206" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10130,7 +10130,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A207" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10162,7 +10162,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A208" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10194,7 +10194,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A209" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10223,7 +10223,7 @@
         <v>0.74999999999999967</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A210" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10255,7 +10255,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A211" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10287,7 +10287,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A212" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10316,7 +10316,7 @@
         <v>2.2499999999999996</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A213" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10351,7 +10351,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A214" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10383,7 +10383,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A215" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10412,7 +10412,7 @@
         <v>1.1249999999999996</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A216" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10444,7 +10444,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A217" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10476,7 +10476,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A218" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10505,7 +10505,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A219" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10540,7 +10540,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A220" s="3" t="str">
         <f t="shared" ref="A220:A229" si="17">A219</f>
         <v>Red</v>
@@ -10578,7 +10578,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A221" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10613,7 +10613,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A222" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10645,7 +10645,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A223" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10680,7 +10680,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A224" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10718,7 +10718,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A225" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10756,7 +10756,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A226" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10791,7 +10791,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A227" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10823,7 +10823,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A228" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10858,7 +10858,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A229" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10896,7 +10896,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A230" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
fixed yardblock, fixed close block, fixed, open block
</commit_message>
<xml_diff>
--- a/TrainProject/Excel Files/TrackLayoutUpdated.xlsx
+++ b/TrainProject/Excel Files/TrackLayoutUpdated.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabe\Documents\TrainProject\TrainProject\Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaitlyn\Desktop\trainproj\TrainProject\TrainProject\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7536" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Red Line" sheetId="1" r:id="rId1"/>
     <sheet name="Green Line" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -465,23 +465,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -517,23 +500,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -717,23 +683,23 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:L78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="3"/>
-    <col min="2" max="2" width="12.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="3"/>
+    <col min="2" max="2" width="12.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" style="3" customWidth="1"/>
-    <col min="8" max="10" width="8.81640625" style="1"/>
-    <col min="11" max="11" width="10.7265625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.26953125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.453125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.81640625" style="1"/>
+    <col min="5" max="5" width="10.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" style="3" customWidth="1"/>
+    <col min="8" max="10" width="8.77734375" style="1"/>
+    <col min="11" max="11" width="10.77734375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -768,7 +734,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -802,7 +768,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Red</v>
@@ -831,7 +797,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A70" si="1">A3</f>
         <v>Red</v>
@@ -863,7 +829,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -895,7 +861,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -924,7 +890,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -956,7 +922,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -991,7 +957,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1020,7 +986,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1058,7 +1024,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1093,7 +1059,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1122,7 +1088,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1154,7 +1120,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1186,7 +1152,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1215,7 +1181,7 @@
         <v>2.0909999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1253,7 +1219,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1291,7 +1257,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1320,7 +1286,7 @@
         <v>0.24099999999999966</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1350,7 +1316,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1379,7 +1345,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1411,7 +1377,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1446,7 +1412,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1475,7 +1441,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1507,7 +1473,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1542,7 +1508,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1574,7 +1540,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1606,7 +1572,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1641,7 +1607,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1676,7 +1642,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1708,7 +1674,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1740,7 +1706,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1772,7 +1738,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1807,7 +1773,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1842,7 +1808,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1874,7 +1840,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1906,7 +1872,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -1938,7 +1904,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Red</v>
@@ -1970,7 +1936,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2005,7 +1971,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2040,7 +2006,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2072,7 +2038,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2104,7 +2070,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2136,7 +2102,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2171,7 +2137,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2206,7 +2172,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2241,7 +2207,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2276,7 +2242,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2308,7 +2274,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2343,7 +2309,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2375,7 +2341,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2404,7 +2370,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2433,7 +2399,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2468,7 +2434,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2500,7 +2466,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2532,7 +2498,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2564,7 +2530,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2593,7 +2559,7 @@
         <v>0.74999999999999967</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2625,7 +2591,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2657,7 +2623,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2686,7 +2652,7 @@
         <v>2.2499999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2721,7 +2687,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2753,7 +2719,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2782,7 +2748,7 @@
         <v>1.1249999999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2814,7 +2780,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2846,7 +2812,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2875,7 +2841,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2910,7 +2876,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2948,7 +2914,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -2983,7 +2949,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Red</v>
@@ -3015,7 +2981,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="str">
         <f t="shared" ref="A71:A77" si="5">A70</f>
         <v>Red</v>
@@ -3050,7 +3016,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3088,7 +3054,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3126,7 +3092,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3161,7 +3127,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3193,7 +3159,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3228,7 +3194,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Red</v>
@@ -3266,7 +3232,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>10</v>
       </c>
@@ -3300,232 +3266,232 @@
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C80" s="5"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" s="5"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="5"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="5"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="5"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" s="5"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" s="5"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C89" s="5"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" s="5"/>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C93" s="5"/>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C94" s="5"/>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C96" s="5"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" s="5"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" s="5"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="5"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="5"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" s="5"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" s="5"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" s="5"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C104" s="5"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C105" s="5"/>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C106" s="5"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C107" s="5"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C108" s="5"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C109" s="5"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C110" s="5"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C111" s="5"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C112" s="5"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C113" s="5"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C114" s="5"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C115" s="5"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C116" s="5"/>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C117" s="5"/>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C118" s="5"/>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C119" s="5"/>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C120" s="5"/>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C121" s="5"/>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C122" s="5"/>
     </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C123" s="5"/>
     </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C124" s="5"/>
     </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C125" s="5"/>
     </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C126" s="5"/>
     </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C127" s="5"/>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C128" s="5"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C129" s="5"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C130" s="5"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C131" s="5"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C132" s="5"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C133" s="5"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C134" s="5"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C135" s="5"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C136" s="5"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C137" s="5"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C138" s="5"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C139" s="5"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C140" s="5"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C141" s="5"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C142" s="5"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C143" s="5"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C144" s="5"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C145" s="5"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C146" s="5"/>
     </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C147" s="5"/>
     </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C148" s="5"/>
     </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C149" s="5"/>
     </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C150" s="5"/>
     </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C151" s="5"/>
     </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C152" s="5"/>
     </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C153" s="5"/>
     </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C154" s="5"/>
     </row>
   </sheetData>
@@ -3539,27 +3505,27 @@
   <dimension ref="A1:L230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G168" sqref="G168"/>
+      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G186" sqref="G186"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="3"/>
-    <col min="2" max="2" width="12.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="3"/>
+    <col min="2" max="2" width="12.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" style="3" customWidth="1"/>
     <col min="7" max="7" width="30" style="3" customWidth="1"/>
-    <col min="8" max="10" width="8.81640625" style="1"/>
-    <col min="11" max="11" width="8.81640625" style="3"/>
-    <col min="12" max="12" width="10.81640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="11.453125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.81640625" style="1"/>
+    <col min="8" max="10" width="8.77734375" style="1"/>
+    <col min="11" max="11" width="8.77734375" style="3"/>
+    <col min="12" max="12" width="10.77734375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="32.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -3594,7 +3560,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -3628,7 +3594,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="str">
         <f>A2</f>
         <v>Green</v>
@@ -3660,7 +3626,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A70" si="1">A3</f>
         <v>Green</v>
@@ -3692,7 +3658,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3724,7 +3690,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3753,7 +3719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3785,7 +3751,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3818,7 +3784,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3847,7 +3813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3879,7 +3845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3908,7 +3874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3937,7 +3903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -3972,7 +3938,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4010,7 +3976,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4039,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4068,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4103,7 +4069,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4135,7 +4101,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4164,7 +4130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4196,7 +4162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4228,7 +4194,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4260,7 +4226,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4292,7 +4258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4321,7 +4287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4350,7 +4316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4379,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4408,7 +4374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4437,7 +4403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4475,7 +4441,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4510,7 +4476,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4539,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4571,7 +4537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4603,7 +4569,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4635,7 +4601,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4664,7 +4630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4696,7 +4662,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4731,7 +4697,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="str">
         <f>A34</f>
         <v>Green</v>
@@ -4763,7 +4729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4795,7 +4761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4827,7 +4793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4859,7 +4825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4891,7 +4857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4923,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4955,7 +4921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -4987,7 +4953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5019,7 +4985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5051,7 +5017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5083,7 +5049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5115,7 +5081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5147,7 +5113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5179,7 +5145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5211,7 +5177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5243,7 +5209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5275,7 +5241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5307,7 +5273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5339,7 +5305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5371,7 +5337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5409,7 +5375,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5445,7 +5411,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5474,7 +5440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5503,7 +5469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5535,7 +5501,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5573,7 +5539,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5605,7 +5571,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5634,7 +5600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5666,7 +5632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5695,7 +5661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5724,7 +5690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5756,7 +5722,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Green</v>
@@ -5788,7 +5754,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="str">
         <f t="shared" ref="A71:A134" si="5">A70</f>
         <v>Green</v>
@@ -5817,7 +5783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5846,7 +5812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5875,7 +5841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5910,7 +5876,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5942,7 +5908,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -5971,7 +5937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6006,7 +5972,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6044,7 +6010,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6073,7 +6039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6102,7 +6068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6131,7 +6097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6160,7 +6126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6189,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6218,7 +6184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6247,7 +6213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6285,7 +6251,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6320,7 +6286,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6349,7 +6315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6384,7 +6350,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6416,7 +6382,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6445,7 +6411,7 @@
         <v>-1.125</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6474,7 +6440,7 @@
         <v>-2.625</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6503,7 +6469,7 @@
         <v>-2.625</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6532,7 +6498,7 @@
         <v>-1.125</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6561,7 +6527,7 @@
         <v>-0.375</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6590,7 +6556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6622,7 +6588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6654,7 +6620,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6686,7 +6652,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6715,7 +6681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6750,7 +6716,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6785,7 +6751,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6817,7 +6783,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6846,7 +6812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6878,7 +6844,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6914,7 +6880,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6943,7 +6909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -6972,7 +6938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7001,7 +6967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7033,7 +6999,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7065,7 +7031,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7094,7 +7060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7123,7 +7089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7152,7 +7118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7185,7 +7151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7214,7 +7180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7246,7 +7212,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7278,7 +7244,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7307,7 +7273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7336,7 +7302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7365,7 +7331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7397,7 +7363,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7432,7 +7398,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7465,7 +7431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7497,7 +7463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7529,7 +7495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7561,7 +7527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7593,7 +7559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7625,7 +7591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7657,7 +7623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7689,7 +7655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7721,7 +7687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7754,7 +7720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="str">
         <f t="shared" si="5"/>
         <v>Green</v>
@@ -7786,7 +7752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="str">
         <f t="shared" ref="A135:A153" si="10">A134</f>
         <v>Green</v>
@@ -7818,7 +7784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7850,7 +7816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7882,7 +7848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7914,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7946,7 +7912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -7978,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8010,7 +7976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8043,7 +8009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8075,7 +8041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8110,7 +8076,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8142,7 +8108,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8171,7 +8137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8203,7 +8169,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8235,7 +8201,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8264,7 +8230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8296,7 +8262,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8331,7 +8297,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8366,7 +8332,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
@@ -8401,7 +8367,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
         <v>10</v>
       </c>
@@ -8435,7 +8401,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="str">
         <f>A154</f>
         <v>Red</v>
@@ -8464,7 +8430,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="str">
         <f t="shared" ref="A156:A219" si="14">A155</f>
         <v>Red</v>
@@ -8496,7 +8462,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8528,7 +8494,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8557,7 +8523,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8589,7 +8555,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8624,7 +8590,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8653,7 +8619,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8691,7 +8657,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8726,7 +8692,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8755,7 +8721,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8787,7 +8753,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8819,7 +8785,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8848,7 +8814,7 @@
         <v>2.0909999999999997</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8883,7 +8849,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="169" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8921,7 +8887,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8950,7 +8916,7 @@
         <v>0.24099999999999966</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8980,7 +8946,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9009,7 +8975,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9041,7 +9007,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9076,7 +9042,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9105,7 +9071,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9137,7 +9103,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9172,7 +9138,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A178" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9204,7 +9170,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9236,7 +9202,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9271,7 +9237,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9306,7 +9272,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9338,7 +9304,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9370,7 +9336,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9402,7 +9368,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9423,7 +9389,7 @@
         <v>70</v>
       </c>
       <c r="G185" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I185" s="8">
         <f t="shared" si="13"/>
@@ -9437,7 +9403,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9458,7 +9424,7 @@
         <v>70</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I186" s="8">
         <f t="shared" si="13"/>
@@ -9472,7 +9438,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9504,7 +9470,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="188" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A188" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9536,7 +9502,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9568,7 +9534,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190" s="3" t="str">
         <f>A186</f>
         <v>Red</v>
@@ -9600,7 +9566,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9635,7 +9601,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A192" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9670,7 +9636,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A193" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9702,7 +9668,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A194" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9734,7 +9700,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A195" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9766,7 +9732,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A196" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9801,7 +9767,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A197" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9836,7 +9802,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="198" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A198" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9871,7 +9837,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A199" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9906,7 +9872,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A200" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9938,7 +9904,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A201" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -9973,7 +9939,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A202" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10005,7 +9971,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A203" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10034,7 +10000,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A204" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10063,7 +10029,7 @@
         <v>-3.3306690738754696E-16</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A205" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10098,7 +10064,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A206" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10130,7 +10096,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A207" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10162,7 +10128,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A208" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10194,7 +10160,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A209" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10223,7 +10189,7 @@
         <v>0.74999999999999967</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10255,7 +10221,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A211" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10287,7 +10253,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A212" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10316,7 +10282,7 @@
         <v>2.2499999999999996</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A213" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10351,7 +10317,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A214" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10383,7 +10349,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A215" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10412,7 +10378,7 @@
         <v>1.1249999999999996</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A216" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10444,7 +10410,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A217" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10476,7 +10442,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A218" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10505,7 +10471,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A219" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -10540,7 +10506,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A220" s="3" t="str">
         <f t="shared" ref="A220:A229" si="17">A219</f>
         <v>Red</v>
@@ -10578,7 +10544,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A221" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10613,7 +10579,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A222" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10645,7 +10611,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A223" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10680,7 +10646,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A224" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10718,7 +10684,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A225" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10756,7 +10722,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A226" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10791,7 +10757,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A227" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10823,7 +10789,7 @@
         <v>-4.4408920985006262E-16</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A228" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10858,7 +10824,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A229" s="3" t="str">
         <f t="shared" si="17"/>
         <v>Red</v>
@@ -10896,7 +10862,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A230" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>